<commit_message>
refactor: Update the project's fill test demo.
</commit_message>
<xml_diff>
--- a/fastexcel-test/src/test/resources/demo/fill/list.xlsx
+++ b/fastexcel-test/src/test/resources/demo/fill/list.xlsx
@@ -1,40 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhuangjiaju/IdeaProjects/easyexcel/src/test/resources/demo/fill/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yanxin/Documents/GitHub/fastexcel/fastexcel-test/src/test/resources/demo/fill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8AB21D-8F7F-7B49-849D-D9F4EE26DEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EA5EFD-A5B9-D648-8A29-1AD92A6F0F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6280" yWindow="780" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>姓名</t>
-  </si>
-  <si>
-    <t>数字</t>
-  </si>
-  <si>
     <t>{.number}</t>
-  </si>
-  <si>
-    <t>日期</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>{.date}</t>
@@ -42,6 +32,18 @@
   </si>
   <si>
     <t>{.name}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -419,7 +421,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -429,25 +431,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>